<commit_message>
Cambios en base de datos
</commit_message>
<xml_diff>
--- a/data/NochipaCloud.xlsx
+++ b/data/NochipaCloud.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erick\Desktop\Universidad\Innovaccion Virtual Microsoft\NochipaCloud\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\NochipaCloud\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCF5F86-9C37-4BF6-A3F4-9B8C40750860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA594571-1F5F-4A53-9243-9112D1C4766B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="238">
   <si>
     <t>Name</t>
   </si>
@@ -75,9 +75,6 @@
     <t>4 Av. Guadalupe Victoria</t>
   </si>
   <si>
-    <t>Bebé</t>
-  </si>
-  <si>
     <t>Niño</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
     <t>Jeans</t>
   </si>
   <si>
-    <t>Pantalones</t>
-  </si>
-  <si>
     <t>CASA PEREZ</t>
   </si>
   <si>
@@ -195,9 +189,6 @@
     <t>10 Av. Guadalupe Victoria</t>
   </si>
   <si>
-    <t>Camisas</t>
-  </si>
-  <si>
     <t>GRISELL</t>
   </si>
   <si>
@@ -207,9 +198,6 @@
     <t>Elegante</t>
   </si>
   <si>
-    <t>Vestidos</t>
-  </si>
-  <si>
     <t>Bombay</t>
   </si>
   <si>
@@ -237,9 +225,6 @@
     <t>21 Av. Álvaro Obregón</t>
   </si>
   <si>
-    <t>Trajes</t>
-  </si>
-  <si>
     <t>Rosse</t>
   </si>
   <si>
@@ -267,9 +252,6 @@
     <t>27 Av. Álvaro Obregón</t>
   </si>
   <si>
-    <t>Chamarras</t>
-  </si>
-  <si>
     <t>Roslov</t>
   </si>
   <si>
@@ -291,12 +273,6 @@
     <t>29 Av. Álvaro Obregón</t>
   </si>
   <si>
-    <t>Cobertores</t>
-  </si>
-  <si>
-    <t>Cobijas</t>
-  </si>
-  <si>
     <t>Rojo Sport</t>
   </si>
   <si>
@@ -525,9 +501,6 @@
     <t>18 Del Gral. José Ma. Magaña</t>
   </si>
   <si>
-    <t>Deportivo</t>
-  </si>
-  <si>
     <t>Futbol</t>
   </si>
   <si>
@@ -588,9 +561,6 @@
     <t>11 C. 5 de Mayo</t>
   </si>
   <si>
-    <t>Zapatos</t>
-  </si>
-  <si>
     <t>Super Dreams</t>
   </si>
   <si>
@@ -705,9 +675,6 @@
     <t>1-A Av. Colón</t>
   </si>
   <si>
-    <t>Pantalón</t>
-  </si>
-  <si>
     <t>The Jean's Home</t>
   </si>
   <si>
@@ -744,18 +711,12 @@
     <t>44 Av. Colón</t>
   </si>
   <si>
-    <t>Sueteres</t>
-  </si>
-  <si>
     <t>Mithos</t>
   </si>
   <si>
     <t>35 Av. Colón</t>
   </si>
   <si>
-    <t>Deportiva</t>
-  </si>
-  <si>
     <t>Gypsy Road</t>
   </si>
   <si>
@@ -769,13 +730,28 @@
   </si>
   <si>
     <t>25 Av. Colón</t>
+  </si>
+  <si>
+    <t>Bebe</t>
+  </si>
+  <si>
+    <t>Vestido</t>
+  </si>
+  <si>
+    <t>Cobertor</t>
+  </si>
+  <si>
+    <t>Cobija</t>
+  </si>
+  <si>
+    <t>Zapato</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -813,6 +789,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -834,13 +818,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1157,8 +1142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1231,13 +1216,13 @@
         <v>-101.18007</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="J2" s="2">
         <v>700</v>
@@ -1248,7 +1233,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>12</v>
@@ -1266,13 +1251,13 @@
         <v>-101.180098</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="J3" s="2">
         <v>600</v>
@@ -1283,13 +1268,13 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="D4">
         <v>38980</v>
@@ -1301,10 +1286,10 @@
         <v>-101.162516676458</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>233</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J4">
         <v>900</v>
@@ -1315,7 +1300,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -1333,10 +1318,10 @@
         <v>-101.18006699999999</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>233</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J5">
         <v>800</v>
@@ -1347,13 +1332,13 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D6">
         <v>38980</v>
@@ -1365,10 +1350,10 @@
         <v>-101.17996100000001</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J6" s="5">
         <v>700</v>
@@ -1379,13 +1364,13 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
         <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
       </c>
       <c r="D7">
         <v>38980</v>
@@ -1397,13 +1382,13 @@
         <v>-101.164812647377</v>
       </c>
       <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" t="s">
         <v>28</v>
-      </c>
-      <c r="H7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" t="s">
-        <v>29</v>
       </c>
       <c r="J7">
         <v>800</v>
@@ -1414,13 +1399,13 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="D8">
         <v>38980</v>
@@ -1432,13 +1417,13 @@
         <v>-101.179863</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J8" s="5">
         <v>800</v>
@@ -1449,13 +1434,13 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D9">
         <v>38980</v>
@@ -1467,13 +1452,13 @@
         <v>-101.17981</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J9" s="5">
         <v>800</v>
@@ -1484,13 +1469,13 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10">
         <v>38980</v>
@@ -1502,13 +1487,13 @@
         <v>-101.17977999999999</v>
       </c>
       <c r="G10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J10" s="5">
         <v>800</v>
@@ -1519,13 +1504,13 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D11">
         <v>38980</v>
@@ -1537,13 +1522,13 @@
         <v>-101.165844174708</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J11">
         <v>800</v>
@@ -1554,13 +1539,13 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D12">
         <v>38980</v>
@@ -1572,13 +1557,13 @@
         <v>-101.17153012728799</v>
       </c>
       <c r="G12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J12">
         <v>830</v>
@@ -1589,13 +1574,13 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D13">
         <v>38980</v>
@@ -1607,13 +1592,13 @@
         <v>-101.167689203991</v>
       </c>
       <c r="G13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J13">
         <v>930</v>
@@ -1624,13 +1609,13 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D14">
         <v>38980</v>
@@ -1642,13 +1627,13 @@
         <v>-101.172023653762</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I14" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="J14">
         <v>900</v>
@@ -1659,13 +1644,13 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D15">
         <v>38980</v>
@@ -1677,13 +1662,13 @@
         <v>-101.17973600000001</v>
       </c>
       <c r="G15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I15" t="s">
-        <v>54</v>
+        <v>122</v>
       </c>
       <c r="J15" s="5">
         <v>600</v>
@@ -1694,13 +1679,13 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D16">
         <v>38980</v>
@@ -1712,13 +1697,13 @@
         <v>-101.179614</v>
       </c>
       <c r="G16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H16" t="s">
-        <v>58</v>
+        <v>234</v>
       </c>
       <c r="I16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J16" s="5">
         <v>700</v>
@@ -1729,13 +1714,13 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D17">
         <v>38980</v>
@@ -1747,13 +1732,13 @@
         <v>-101.17945400000001</v>
       </c>
       <c r="G17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H17" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="I17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J17" s="5">
         <v>800</v>
@@ -1764,13 +1749,13 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D18">
         <v>38980</v>
@@ -1782,13 +1767,13 @@
         <v>-101.179485</v>
       </c>
       <c r="G18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J18" s="5">
         <v>700</v>
@@ -1799,13 +1784,13 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D19">
         <v>38980</v>
@@ -1817,13 +1802,13 @@
         <v>-101.17907099999999</v>
       </c>
       <c r="G19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H19" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="I19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J19" s="5">
         <v>700</v>
@@ -1834,13 +1819,13 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D20">
         <v>38980</v>
@@ -1852,13 +1837,13 @@
         <v>-101.179022</v>
       </c>
       <c r="G20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H20" t="s">
-        <v>68</v>
+        <v>194</v>
       </c>
       <c r="I20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J20" s="5">
         <v>800</v>
@@ -1869,13 +1854,13 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D21">
         <v>38980</v>
@@ -1887,10 +1872,10 @@
         <v>-101.178996</v>
       </c>
       <c r="G21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J21" s="5">
         <v>800</v>
@@ -1901,13 +1886,13 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D22">
         <v>38980</v>
@@ -1919,13 +1904,13 @@
         <v>-101.17898599999999</v>
       </c>
       <c r="G22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J22" s="5">
         <v>800</v>
@@ -1936,13 +1921,13 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B23" t="s">
         <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D23">
         <v>38980</v>
@@ -1954,13 +1939,13 @@
         <v>-101.173322575711</v>
       </c>
       <c r="G23" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="H23" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="I23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J23">
         <v>930</v>
@@ -1971,13 +1956,13 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D24">
         <v>38980</v>
@@ -1989,13 +1974,13 @@
         <v>-101.178955</v>
       </c>
       <c r="G24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I24" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="J24" s="5">
         <v>800</v>
@@ -2006,13 +1991,13 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s">
         <v>12</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D25">
         <v>38980</v>
@@ -2024,13 +2009,13 @@
         <v>-101.178955</v>
       </c>
       <c r="G25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J25" s="5">
         <v>800</v>
@@ -2041,13 +2026,13 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
         <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D26">
         <v>38980</v>
@@ -2059,13 +2044,13 @@
         <v>-101.173526423602</v>
       </c>
       <c r="G26" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I26" t="s">
-        <v>54</v>
+        <v>122</v>
       </c>
       <c r="J26">
         <v>900</v>
@@ -2076,13 +2061,13 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B27" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D27">
         <v>38980</v>
@@ -2094,10 +2079,10 @@
         <v>-101.178944</v>
       </c>
       <c r="G27" t="s">
-        <v>86</v>
+        <v>235</v>
       </c>
       <c r="H27" t="s">
-        <v>87</v>
+        <v>236</v>
       </c>
       <c r="J27" s="5">
         <v>600</v>
@@ -2108,13 +2093,13 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B28" t="s">
         <v>12</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D28">
         <v>38980</v>
@@ -2126,13 +2111,13 @@
         <v>-101.178928</v>
       </c>
       <c r="G28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J28" s="5">
         <v>800</v>
@@ -2143,13 +2128,13 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B29" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D29">
         <v>38980</v>
@@ -2161,10 +2146,10 @@
         <v>-101.17889</v>
       </c>
       <c r="G29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" t="s">
         <v>15</v>
-      </c>
-      <c r="H29" t="s">
-        <v>16</v>
       </c>
       <c r="J29" s="5">
         <v>800</v>
@@ -2175,13 +2160,13 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B30" t="s">
         <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D30">
         <v>38980</v>
@@ -2193,10 +2178,10 @@
         <v>-101.17454566297801</v>
       </c>
       <c r="G30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J30">
         <v>900</v>
@@ -2207,13 +2192,13 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B31" t="s">
         <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D31">
         <v>38980</v>
@@ -2225,13 +2210,13 @@
         <v>-101.175650733125</v>
       </c>
       <c r="G31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H31" t="s">
-        <v>58</v>
+        <v>234</v>
       </c>
       <c r="I31" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="J31">
         <v>800</v>
@@ -2242,13 +2227,13 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B32" t="s">
         <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D32">
         <v>38980</v>
@@ -2260,13 +2245,13 @@
         <v>-101.176605599563</v>
       </c>
       <c r="G32" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I32" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="J32">
         <v>800</v>
@@ -2277,13 +2262,13 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B33" t="s">
         <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D33">
         <v>38980</v>
@@ -2295,13 +2280,13 @@
         <v>-101.17526449496501</v>
       </c>
       <c r="G33" t="s">
+        <v>27</v>
+      </c>
+      <c r="H33" t="s">
         <v>28</v>
       </c>
-      <c r="H33" t="s">
-        <v>29</v>
-      </c>
       <c r="I33" t="s">
-        <v>54</v>
+        <v>122</v>
       </c>
       <c r="J33">
         <v>800</v>
@@ -2312,13 +2297,13 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B34" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D34">
         <v>38980</v>
@@ -2330,13 +2315,13 @@
         <v>-101.17889</v>
       </c>
       <c r="G34" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="H34" t="s">
+        <v>27</v>
+      </c>
+      <c r="I34" t="s">
         <v>28</v>
-      </c>
-      <c r="I34" t="s">
-        <v>29</v>
       </c>
       <c r="J34" s="5">
         <v>800</v>
@@ -2347,13 +2332,13 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B35" t="s">
         <v>12</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D35">
         <v>38980</v>
@@ -2365,13 +2350,13 @@
         <v>-101.17887</v>
       </c>
       <c r="G35" t="s">
-        <v>58</v>
+        <v>234</v>
       </c>
       <c r="H35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J35" s="5">
         <v>800</v>
@@ -2382,13 +2367,13 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B36" t="s">
         <v>12</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D36">
         <v>38980</v>
@@ -2400,13 +2385,13 @@
         <v>-101.178822</v>
       </c>
       <c r="G36" t="s">
+        <v>27</v>
+      </c>
+      <c r="H36" t="s">
         <v>28</v>
       </c>
-      <c r="H36" t="s">
-        <v>29</v>
-      </c>
       <c r="I36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J36" s="5">
         <v>800</v>
@@ -2417,13 +2402,13 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B37" t="s">
         <v>12</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D37">
         <v>38980</v>
@@ -2435,10 +2420,10 @@
         <v>-101.17880700000001</v>
       </c>
       <c r="G37" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="I37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J37">
         <v>930</v>
@@ -2449,13 +2434,13 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B38" t="s">
         <v>12</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D38">
         <v>38980</v>
@@ -2467,13 +2452,13 @@
         <v>-101.17879499999999</v>
       </c>
       <c r="G38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H38" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="I38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J38">
         <v>930</v>
@@ -2484,13 +2469,13 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B39" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C39" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D39">
         <v>38940</v>
@@ -2502,13 +2487,13 @@
         <v>-101.12862111120199</v>
       </c>
       <c r="G39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H39" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="I39" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J39">
         <v>1000</v>
@@ -2519,13 +2504,13 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B40" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C40" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D40">
         <v>38940</v>
@@ -2537,13 +2522,13 @@
         <v>-101.13643170408599</v>
       </c>
       <c r="G40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H40" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I40" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J40">
         <v>800</v>
@@ -2554,13 +2539,13 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B41" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C41" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D41">
         <v>38940</v>
@@ -2572,13 +2557,13 @@
         <v>-101.12982274087599</v>
       </c>
       <c r="G41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H41" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I41" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J41">
         <v>900</v>
@@ -2589,13 +2574,13 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B42" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C42" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D42">
         <v>38940</v>
@@ -2607,13 +2592,13 @@
         <v>-101.137633333761</v>
       </c>
       <c r="G42" t="s">
-        <v>54</v>
+        <v>122</v>
       </c>
       <c r="H42" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J42">
         <v>900</v>
@@ -2624,13 +2609,13 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B43" t="s">
         <v>12</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D43">
         <v>38980</v>
@@ -2642,13 +2627,13 @@
         <v>-101.178786</v>
       </c>
       <c r="G43" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J43" s="5">
         <v>800</v>
@@ -2659,13 +2644,13 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B44" t="s">
         <v>12</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D44">
         <v>38980</v>
@@ -2677,10 +2662,10 @@
         <v>-101.179148</v>
       </c>
       <c r="G44" t="s">
-        <v>58</v>
+        <v>234</v>
       </c>
       <c r="H44" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="J44" s="5">
         <v>800</v>
@@ -2691,13 +2676,13 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B45" t="s">
         <v>12</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D45">
         <v>38980</v>
@@ -2709,13 +2694,13 @@
         <v>-101.17876800000001</v>
       </c>
       <c r="G45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I45" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="J45" s="5">
         <v>800</v>
@@ -2726,13 +2711,13 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B46" t="s">
         <v>12</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D46">
         <v>38980</v>
@@ -2744,13 +2729,13 @@
         <v>-101.178755</v>
       </c>
       <c r="G46" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I46" t="s">
-        <v>54</v>
+        <v>122</v>
       </c>
       <c r="J46">
         <v>930</v>
@@ -2761,13 +2746,13 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B47" t="s">
         <v>12</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D47">
         <v>38980</v>
@@ -2779,13 +2764,13 @@
         <v>-101.178844754922</v>
       </c>
       <c r="G47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H47" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="I47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J47" s="5">
         <v>800</v>
@@ -2796,13 +2781,13 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B48" t="s">
         <v>12</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D48">
         <v>38980</v>
@@ -2814,10 +2799,10 @@
         <v>-101.178797677623</v>
       </c>
       <c r="G48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J48" s="5">
         <v>800</v>
@@ -2828,13 +2813,13 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B49" t="s">
         <v>12</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D49">
         <v>38980</v>
@@ -2846,13 +2831,13 @@
         <v>-101.178805724253</v>
       </c>
       <c r="G49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J49">
         <v>1000</v>
@@ -2863,13 +2848,13 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B50" t="s">
         <v>12</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D50">
         <v>38980</v>
@@ -2881,13 +2866,13 @@
         <v>-101.17861260519901</v>
       </c>
       <c r="G50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H50" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I50" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="J50">
         <v>800</v>
@@ -2898,13 +2883,13 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B51" t="s">
         <v>12</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D51">
         <v>38980</v>
@@ -2916,10 +2901,10 @@
         <v>-101.17835913644799</v>
       </c>
       <c r="G51" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="H51" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="J51">
         <v>800</v>
@@ -2930,13 +2915,13 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B52" t="s">
         <v>12</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D52">
         <v>38980</v>
@@ -2948,13 +2933,13 @@
         <v>-101.17760836890901</v>
       </c>
       <c r="G52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H52" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J52" s="5">
         <v>800</v>
@@ -2965,13 +2950,13 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B53" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C53" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D53">
         <v>38940</v>
@@ -2983,10 +2968,10 @@
         <v>-101.14080906932899</v>
       </c>
       <c r="G53" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="H53" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="J53">
         <v>930</v>
@@ -2997,13 +2982,13 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B54" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C54" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D54">
         <v>38940</v>
@@ -3015,13 +3000,13 @@
         <v>-101.121668825228</v>
       </c>
       <c r="G54" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H54" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="I54" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J54">
         <v>1100</v>
@@ -3032,13 +3017,13 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C55" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D55">
         <v>38940</v>
@@ -3050,13 +3035,13 @@
         <v>-101.121668825228</v>
       </c>
       <c r="G55" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="H55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I55" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J55">
         <v>1000</v>
@@ -3067,13 +3052,13 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B56" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C56" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D56">
         <v>38940</v>
@@ -3085,13 +3070,13 @@
         <v>-101.12862111120199</v>
       </c>
       <c r="G56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H56" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="I56" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J56">
         <v>1000</v>
@@ -3102,13 +3087,13 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B57" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C57" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D57">
         <v>38940</v>
@@ -3120,13 +3105,13 @@
         <v>-101.130509386405</v>
       </c>
       <c r="G57" t="s">
+        <v>233</v>
+      </c>
+      <c r="H57" t="s">
+        <v>15</v>
+      </c>
+      <c r="I57" t="s">
         <v>14</v>
-      </c>
-      <c r="H57" t="s">
-        <v>16</v>
-      </c>
-      <c r="I57" t="s">
-        <v>15</v>
       </c>
       <c r="J57">
         <v>1000</v>
@@ -3137,13 +3122,13 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B58" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C58" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D58">
         <v>38940</v>
@@ -3155,13 +3140,13 @@
         <v>-101.129479418112</v>
       </c>
       <c r="G58" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H58" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I58" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="J58">
         <v>1000</v>
@@ -3172,13 +3157,13 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B59" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C59" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D59">
         <v>38940</v>
@@ -3190,13 +3175,13 @@
         <v>-101.1334276299</v>
       </c>
       <c r="G59" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H59" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I59" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="J59">
         <v>1000</v>
@@ -3207,13 +3192,13 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B60" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C60" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D60">
         <v>38940</v>
@@ -3225,13 +3210,13 @@
         <v>-101.129651079494</v>
       </c>
       <c r="G60" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H60" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I60" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="J60">
         <v>1000</v>
@@ -3242,13 +3227,13 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B61" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C61" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="D61">
         <v>38940</v>
@@ -3260,13 +3245,13 @@
         <v>-101.12939358742101</v>
       </c>
       <c r="G61" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H61" t="s">
-        <v>164</v>
+        <v>17</v>
       </c>
       <c r="I61" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="J61">
         <v>1000</v>
@@ -3277,13 +3262,13 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B62" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C62" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="D62">
         <v>38940</v>
@@ -3295,13 +3280,13 @@
         <v>-101.127896572737</v>
       </c>
       <c r="G62" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H62" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I62" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="J62">
         <v>1000</v>
@@ -3312,13 +3297,13 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B63" t="s">
         <v>12</v>
       </c>
       <c r="C63" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="D63">
         <v>38980</v>
@@ -3330,13 +3315,13 @@
         <v>-101.183659832155</v>
       </c>
       <c r="G63" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H63" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I63" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="J63">
         <v>900</v>
@@ -3347,13 +3332,13 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B64" t="s">
         <v>12</v>
       </c>
       <c r="C64" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D64">
         <v>38980</v>
@@ -3365,13 +3350,13 @@
         <v>-101.18364149091499</v>
       </c>
       <c r="G64" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H64" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I64" t="s">
-        <v>54</v>
+        <v>122</v>
       </c>
       <c r="J64">
         <v>900</v>
@@ -3382,13 +3367,13 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B65" t="s">
         <v>12</v>
       </c>
       <c r="C65" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="D65">
         <v>38980</v>
@@ -3400,10 +3385,10 @@
         <v>-101.18377154698599</v>
       </c>
       <c r="H65" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I65" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J65">
         <v>900</v>
@@ -3414,13 +3399,13 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B66" t="s">
         <v>12</v>
       </c>
       <c r="C66" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="D66">
         <v>38980</v>
@@ -3432,13 +3417,13 @@
         <v>-101.183888263969</v>
       </c>
       <c r="G66" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H66" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I66" t="s">
-        <v>54</v>
+        <v>122</v>
       </c>
       <c r="J66">
         <v>900</v>
@@ -3449,13 +3434,13 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B67" t="s">
         <v>12</v>
       </c>
       <c r="C67" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D67">
         <v>38980</v>
@@ -3467,10 +3452,10 @@
         <v>-101.18400831572301</v>
       </c>
       <c r="G67" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H67" t="s">
-        <v>58</v>
+        <v>234</v>
       </c>
       <c r="J67">
         <v>500</v>
@@ -3481,13 +3466,13 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B68" t="s">
         <v>12</v>
       </c>
       <c r="C68" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="D68">
         <v>38980</v>
@@ -3499,10 +3484,10 @@
         <v>-101.18392911491</v>
       </c>
       <c r="G68" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H68" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J68">
         <v>1000</v>
@@ -3513,13 +3498,13 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B69" t="s">
         <v>12</v>
       </c>
       <c r="C69" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="D69">
         <v>38980</v>
@@ -3531,7 +3516,7 @@
         <v>-101.18406917529001</v>
       </c>
       <c r="G69" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J69">
         <v>930</v>
@@ -3542,13 +3527,13 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B70" t="s">
         <v>12</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="D70">
         <v>38980</v>
@@ -3560,13 +3545,13 @@
         <v>-101.179896391954</v>
       </c>
       <c r="G70" t="s">
-        <v>185</v>
+        <v>237</v>
       </c>
       <c r="H70" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I70" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J70" s="5">
         <v>800</v>
@@ -3577,13 +3562,13 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B71" t="s">
         <v>12</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="D71">
         <v>38980</v>
@@ -3595,13 +3580,13 @@
         <v>-101.180469812243</v>
       </c>
       <c r="G71" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="H71" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I71" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J71">
         <v>1000</v>
@@ -3612,13 +3597,13 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="B72" t="s">
         <v>12</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="D72">
         <v>38980</v>
@@ -3630,13 +3615,13 @@
         <v>-101.18069211780301</v>
       </c>
       <c r="G72" t="s">
+        <v>14</v>
+      </c>
+      <c r="H72" t="s">
         <v>15</v>
       </c>
-      <c r="H72" t="s">
-        <v>16</v>
-      </c>
       <c r="I72" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="J72" s="5">
         <v>800</v>
@@ -3647,13 +3632,13 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="B73" t="s">
         <v>12</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="D73">
         <v>38980</v>
@@ -3665,13 +3650,13 @@
         <v>-101.18080208837</v>
       </c>
       <c r="G73" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H73" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="I73" t="s">
-        <v>54</v>
+        <v>122</v>
       </c>
       <c r="J73" s="5">
         <v>800</v>
@@ -3682,13 +3667,13 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="B74" t="s">
         <v>12</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="D74">
         <v>38980</v>
@@ -3700,13 +3685,13 @@
         <v>-101.181068967161</v>
       </c>
       <c r="G74" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H74" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="I74" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J74">
         <v>930</v>
@@ -3717,13 +3702,13 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="B75" t="s">
         <v>12</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="D75">
         <v>38980</v>
@@ -3735,13 +3720,13 @@
         <v>-101.181579469422</v>
       </c>
       <c r="G75" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H75" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I75" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="J75" s="5">
         <v>800</v>
@@ -3752,13 +3737,13 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="B76" t="s">
         <v>12</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="D76">
         <v>38980</v>
@@ -3770,13 +3755,13 @@
         <v>-101.182169701493</v>
       </c>
       <c r="G76" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="H76" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I76" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J76" s="5">
         <v>800</v>
@@ -3787,13 +3772,13 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B77" t="s">
         <v>12</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="D77">
         <v>38980</v>
@@ -3805,13 +3790,13 @@
         <v>-101.18229853806901</v>
       </c>
       <c r="G77" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H77" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I77" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="J77" s="5">
         <v>800</v>
@@ -3822,13 +3807,13 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="B78" t="s">
         <v>12</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="D78">
         <v>38980</v>
@@ -3840,13 +3825,13 @@
         <v>-101.182583197955</v>
       </c>
       <c r="G78" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H78" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="I78" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="J78">
         <v>930</v>
@@ -3857,13 +3842,13 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="B79" t="s">
         <v>12</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="D79">
         <v>38980</v>
@@ -3875,7 +3860,7 @@
         <v>-101.182948193024</v>
       </c>
       <c r="G79" t="s">
-        <v>185</v>
+        <v>237</v>
       </c>
       <c r="J79">
         <v>800</v>
@@ -3886,13 +3871,13 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="B80" t="s">
         <v>12</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="D80">
         <v>38980</v>
@@ -3904,13 +3889,13 @@
         <v>-101.18310296151</v>
       </c>
       <c r="G80" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H80" t="s">
-        <v>54</v>
+        <v>122</v>
       </c>
       <c r="I80" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="J80">
         <v>800</v>
@@ -3921,13 +3906,13 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="B81" t="s">
         <v>12</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="D81">
         <v>38980</v>
@@ -3939,13 +3924,13 @@
         <v>-101.18324251076599</v>
       </c>
       <c r="G81" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="H81" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="I81" t="s">
-        <v>185</v>
+        <v>237</v>
       </c>
       <c r="J81">
         <v>1000</v>
@@ -3956,13 +3941,13 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="B82" t="s">
         <v>12</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="D82">
         <v>38980</v>
@@ -3974,13 +3959,13 @@
         <v>-101.183363445056</v>
       </c>
       <c r="G82" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="H82" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="I82" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="J82">
         <v>800</v>
@@ -3991,13 +3976,13 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="D83">
         <v>38800</v>
@@ -4009,13 +3994,13 @@
         <v>-101.18462834144999</v>
       </c>
       <c r="G83" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H83" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="I83" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="J83">
         <v>800</v>
@@ -4026,13 +4011,13 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="D84">
         <v>38800</v>
@@ -4044,13 +4029,13 @@
         <v>-101.184952025664</v>
       </c>
       <c r="G84" t="s">
-        <v>58</v>
+        <v>234</v>
       </c>
       <c r="H84" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="I84" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J84">
         <v>1000</v>
@@ -4061,13 +4046,13 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="D85">
         <v>38800</v>
@@ -4079,13 +4064,13 @@
         <v>-101.185672848983</v>
       </c>
       <c r="G85" t="s">
-        <v>58</v>
+        <v>234</v>
       </c>
       <c r="H85" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I85" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J85">
         <v>1000</v>
@@ -4096,13 +4081,13 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="D86">
         <v>38800</v>
@@ -4114,13 +4099,13 @@
         <v>-101.18579891281099</v>
       </c>
       <c r="G86" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="H86" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="I86" t="s">
-        <v>224</v>
+        <v>34</v>
       </c>
       <c r="J86">
         <v>800</v>
@@ -4131,13 +4116,13 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="D87">
         <v>38800</v>
@@ -4149,7 +4134,10 @@
         <v>-101.18700121671699</v>
       </c>
       <c r="G87" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="H87" t="s">
+        <v>70</v>
       </c>
       <c r="J87">
         <v>800</v>
@@ -4160,13 +4148,13 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="D88">
         <v>38800</v>
@@ -4177,11 +4165,14 @@
       <c r="F88">
         <v>-101.186381626404</v>
       </c>
+      <c r="G88" t="s">
+        <v>17</v>
+      </c>
       <c r="H88" t="s">
-        <v>14</v>
+        <v>233</v>
       </c>
       <c r="I88" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="J88">
         <v>1000</v>
@@ -4192,13 +4183,13 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C89" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="D89">
         <v>38800</v>
@@ -4210,7 +4201,7 @@
         <v>-101.186032939238</v>
       </c>
       <c r="G89" t="s">
-        <v>14</v>
+        <v>233</v>
       </c>
       <c r="J89">
         <v>800</v>
@@ -4221,13 +4212,13 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="D90">
         <v>38800</v>
@@ -4239,13 +4230,13 @@
         <v>-101.186124134349</v>
       </c>
       <c r="G90" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H90" t="s">
-        <v>58</v>
+        <v>234</v>
       </c>
       <c r="I90" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="J90">
         <v>800</v>
@@ -4256,13 +4247,13 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="D91">
         <v>38800</v>
@@ -4274,13 +4265,13 @@
         <v>-101.185284048638</v>
       </c>
       <c r="G91" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H91" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I91" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J91">
         <v>900</v>
@@ -4291,13 +4282,13 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="B92" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C92" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="D92">
         <v>38800</v>
@@ -4309,13 +4300,13 @@
         <v>-101.184050000356</v>
       </c>
       <c r="G92" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H92" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="I92" t="s">
-        <v>237</v>
+        <v>31</v>
       </c>
       <c r="J92">
         <v>900</v>
@@ -4326,13 +4317,13 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="B93" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C93" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="D93">
         <v>38800</v>
@@ -4344,13 +4335,13 @@
         <v>-101.18423758122201</v>
       </c>
       <c r="G93" t="s">
-        <v>240</v>
+        <v>17</v>
       </c>
       <c r="H93" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I93" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J93">
         <v>930</v>
@@ -4361,13 +4352,13 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="B94" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C94" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="D94">
         <v>38800</v>
@@ -4379,10 +4370,10 @@
         <v>-101.18425258769</v>
       </c>
       <c r="G94" t="s">
-        <v>240</v>
+        <v>17</v>
       </c>
       <c r="H94" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J94">
         <v>1000</v>
@@ -4393,13 +4384,13 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="B95" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C95" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="D95">
         <v>38800</v>
@@ -4411,7 +4402,7 @@
         <v>-101.18437930898899</v>
       </c>
       <c r="G95" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J95">
         <v>900</v>
@@ -4422,13 +4413,13 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="B96" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C96" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="D96">
         <v>38800</v>
@@ -4440,10 +4431,10 @@
         <v>-101.1843893133</v>
       </c>
       <c r="G96" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H96" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J96">
         <v>900</v>
@@ -4454,5 +4445,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>